<commit_message>
feat(import): Añadir importación masiva y corregir creación de recursos
Se introduce una funcionalidad para importar usuarios, libros y recursos desde archivos Excel. Adicionalmente, se corrige un error en la creación manual de recursos.

- Backend: Se añade un nuevo controlador (importController), rutas (/api/import) y middleware (multer) para manejar la subida y procesamiento de archivos.

- Frontend: Se crea un componente reutilizable (ImportComponent) para la carga de archivos, descarga de plantillas y visualización de resultados.

- fix(resources): Se corrige la función createResource en esourceController.js para manejar correctamente los datos anidados del formulario, solucionando un error de clave duplicada.
</commit_message>
<xml_diff>
--- a/frontend/public/templates/plantilla_recursos.xlsx
+++ b/frontend/public/templates/plantilla_recursos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\Desktop\Proyecto de Título\Documentos Apoyo\Plantilas Importacion Masiva\Ejemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4547CF8-8C9D-4632-828B-446395A80E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFD98A4-A797-4331-957B-113D2376C76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42870" yWindow="4860" windowWidth="22485" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11220" yWindow="10110" windowWidth="22485" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plantilla_libros.xlsx_x000a_Obligator" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>ubicacion</t>
   </si>
   <si>
-    <t>Set de Ajedrez de Madera</t>
-  </si>
-  <si>
     <t>juego</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>Estante de Juegos</t>
+  </si>
+  <si>
+    <t>Madera</t>
   </si>
 </sst>
 </file>
@@ -322,9 +322,18 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -351,25 +360,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>